<commit_message>
Update the scenario ID in the employment by MSA based on SR14 preliminary forecast.
</commit_message>
<xml_diff>
--- a/off_model_calculators/sandag_inputs/emp_msa_preliminarySR14.xlsx
+++ b/off_model_calculators/sandag_inputs/emp_msa_preliminarySR14.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\RES\TransModel\2019RTP\off_model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A646A864-B77B-4AA9-82ED-75F4DEA25C13}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{394E27BE-B11E-4031-9910-3D5D3996FB01}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="10095" xr2:uid="{2A89E2C9-F974-4C74-B59E-A596A1BE5ECE}"/>
   </bookViews>
@@ -531,7 +531,7 @@
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E2" sqref="E2"/>
+      <selection pane="bottomRight" activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -651,7 +651,7 @@
         <v>2016</v>
       </c>
       <c r="B2" s="3">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="C2" s="3">
         <v>0</v>
@@ -761,7 +761,7 @@
         <v>2016</v>
       </c>
       <c r="B3" s="3">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="C3" s="3">
         <v>1</v>
@@ -871,7 +871,7 @@
         <v>2016</v>
       </c>
       <c r="B4" s="3">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="C4" s="3">
         <v>2</v>
@@ -981,7 +981,7 @@
         <v>2016</v>
       </c>
       <c r="B5" s="3">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="C5" s="3">
         <v>3</v>
@@ -1091,7 +1091,7 @@
         <v>2016</v>
       </c>
       <c r="B6" s="3">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="C6" s="3">
         <v>4</v>
@@ -1201,7 +1201,7 @@
         <v>2016</v>
       </c>
       <c r="B7" s="3">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="C7" s="3">
         <v>5</v>
@@ -1311,7 +1311,7 @@
         <v>2016</v>
       </c>
       <c r="B8" s="3">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="C8" s="3">
         <v>6</v>
@@ -1421,7 +1421,7 @@
         <v>2020</v>
       </c>
       <c r="B9">
-        <v>82</v>
+        <v>101</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -1530,8 +1530,8 @@
       <c r="A10" s="2">
         <v>2020</v>
       </c>
-      <c r="B10">
-        <v>82</v>
+      <c r="B10" s="2">
+        <v>101</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -1640,8 +1640,8 @@
       <c r="A11" s="2">
         <v>2020</v>
       </c>
-      <c r="B11">
-        <v>82</v>
+      <c r="B11" s="2">
+        <v>101</v>
       </c>
       <c r="C11">
         <v>2</v>
@@ -1750,8 +1750,8 @@
       <c r="A12" s="2">
         <v>2020</v>
       </c>
-      <c r="B12">
-        <v>82</v>
+      <c r="B12" s="2">
+        <v>101</v>
       </c>
       <c r="C12">
         <v>3</v>
@@ -1860,8 +1860,8 @@
       <c r="A13" s="2">
         <v>2020</v>
       </c>
-      <c r="B13">
-        <v>82</v>
+      <c r="B13" s="2">
+        <v>101</v>
       </c>
       <c r="C13">
         <v>4</v>
@@ -1970,8 +1970,8 @@
       <c r="A14" s="2">
         <v>2020</v>
       </c>
-      <c r="B14">
-        <v>82</v>
+      <c r="B14" s="2">
+        <v>101</v>
       </c>
       <c r="C14">
         <v>5</v>
@@ -2080,8 +2080,8 @@
       <c r="A15" s="2">
         <v>2020</v>
       </c>
-      <c r="B15">
-        <v>82</v>
+      <c r="B15" s="2">
+        <v>101</v>
       </c>
       <c r="C15">
         <v>6</v>
@@ -2191,7 +2191,7 @@
         <v>2025</v>
       </c>
       <c r="B16" s="3">
-        <v>81</v>
+        <v>102</v>
       </c>
       <c r="C16" s="3">
         <v>0</v>
@@ -2301,7 +2301,7 @@
         <v>2025</v>
       </c>
       <c r="B17" s="3">
-        <v>81</v>
+        <v>102</v>
       </c>
       <c r="C17" s="3">
         <v>1</v>
@@ -2411,7 +2411,7 @@
         <v>2025</v>
       </c>
       <c r="B18" s="3">
-        <v>81</v>
+        <v>102</v>
       </c>
       <c r="C18" s="3">
         <v>2</v>
@@ -2521,7 +2521,7 @@
         <v>2025</v>
       </c>
       <c r="B19" s="3">
-        <v>81</v>
+        <v>102</v>
       </c>
       <c r="C19" s="3">
         <v>3</v>
@@ -2631,7 +2631,7 @@
         <v>2025</v>
       </c>
       <c r="B20" s="3">
-        <v>81</v>
+        <v>102</v>
       </c>
       <c r="C20" s="3">
         <v>4</v>
@@ -2741,7 +2741,7 @@
         <v>2025</v>
       </c>
       <c r="B21" s="3">
-        <v>81</v>
+        <v>102</v>
       </c>
       <c r="C21" s="3">
         <v>5</v>
@@ -2851,7 +2851,7 @@
         <v>2025</v>
       </c>
       <c r="B22" s="3">
-        <v>81</v>
+        <v>102</v>
       </c>
       <c r="C22" s="3">
         <v>6</v>
@@ -2961,7 +2961,7 @@
         <v>2035</v>
       </c>
       <c r="B23">
-        <v>76</v>
+        <v>104</v>
       </c>
       <c r="C23">
         <v>0</v>
@@ -3070,8 +3070,8 @@
       <c r="A24" s="2">
         <v>2035</v>
       </c>
-      <c r="B24">
-        <v>76</v>
+      <c r="B24" s="2">
+        <v>104</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -3180,8 +3180,8 @@
       <c r="A25" s="2">
         <v>2035</v>
       </c>
-      <c r="B25">
-        <v>76</v>
+      <c r="B25" s="2">
+        <v>104</v>
       </c>
       <c r="C25">
         <v>2</v>
@@ -3290,8 +3290,8 @@
       <c r="A26" s="2">
         <v>2035</v>
       </c>
-      <c r="B26">
-        <v>76</v>
+      <c r="B26" s="2">
+        <v>104</v>
       </c>
       <c r="C26">
         <v>3</v>
@@ -3400,8 +3400,8 @@
       <c r="A27" s="2">
         <v>2035</v>
       </c>
-      <c r="B27">
-        <v>76</v>
+      <c r="B27" s="2">
+        <v>104</v>
       </c>
       <c r="C27">
         <v>4</v>
@@ -3510,8 +3510,8 @@
       <c r="A28" s="2">
         <v>2035</v>
       </c>
-      <c r="B28">
-        <v>76</v>
+      <c r="B28" s="2">
+        <v>104</v>
       </c>
       <c r="C28">
         <v>5</v>
@@ -3620,8 +3620,8 @@
       <c r="A29" s="2">
         <v>2035</v>
       </c>
-      <c r="B29">
-        <v>76</v>
+      <c r="B29" s="2">
+        <v>104</v>
       </c>
       <c r="C29">
         <v>6</v>

</xml_diff>